<commit_message>
More stuff done, more to be done
</commit_message>
<xml_diff>
--- a/msmnt_baseline-report.xlsx
+++ b/msmnt_baseline-report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="18855" windowHeight="7875" activeTab="5"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="18855" windowHeight="7875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="baseline-A" sheetId="3" r:id="rId1"/>
@@ -444,9 +444,6 @@
     <t>3 (March 31)</t>
   </si>
   <si>
-    <t>(April 2)</t>
-  </si>
-  <si>
     <t>13 (April 2)</t>
   </si>
   <si>
@@ -477,9 +474,6 @@
     <t>01 (March 11)</t>
   </si>
   <si>
-    <t>(April 1)</t>
-  </si>
-  <si>
     <t>09 (March 23)</t>
   </si>
   <si>
@@ -499,6 +493,12 @@
   </si>
   <si>
     <t>15 (March 31)</t>
+  </si>
+  <si>
+    <t>16 (April 1)</t>
+  </si>
+  <si>
+    <t>17 (April 2)</t>
   </si>
 </sst>
 </file>
@@ -2690,7 +2690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -3569,7 +3569,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3589,7 +3589,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3609,7 +3609,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3629,7 +3629,7 @@
         <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3649,7 +3649,7 @@
         <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3669,7 +3669,7 @@
         <v>60</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3689,7 +3689,7 @@
         <v>64</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3709,7 +3709,7 @@
         <v>73</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3729,7 +3729,7 @@
         <v>77</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3749,7 +3749,7 @@
         <v>82</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3829,7 +3829,7 @@
         <v>107</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3956,8 +3956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3972,30 +3972,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -4004,78 +4004,78 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>109</v>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
@@ -4084,275 +4084,275 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>28</v>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>54</v>
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>50</v>
@@ -4364,10 +4364,10 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4375,19 +4375,19 @@
         <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4398,124 +4398,124 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>10</v>
@@ -4524,55 +4524,55 @@
         <v>3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>27</v>
@@ -4584,90 +4584,90 @@
         <v>31</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4675,16 +4675,16 @@
         <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>152</v>
@@ -4692,19 +4692,19 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>152</v>
@@ -4721,10 +4721,10 @@
         <v>43</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>153</v>
@@ -4744,7 +4744,7 @@
         <v>3</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>153</v>
@@ -4752,19 +4752,19 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>153</v>
@@ -4772,39 +4772,39 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>154</v>
@@ -4812,19 +4812,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>154</v>
@@ -4838,13 +4838,13 @@
         <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>155</v>
@@ -4855,7 +4855,7 @@
         <v>33</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>2</v>
@@ -4864,7 +4864,7 @@
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>155</v>
@@ -4875,16 +4875,16 @@
         <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>155</v>
@@ -4895,16 +4895,16 @@
         <v>26</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>156</v>
@@ -4915,16 +4915,16 @@
         <v>33</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>156</v>
@@ -4935,7 +4935,7 @@
         <v>29</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>2</v>
@@ -4944,7 +4944,7 @@
         <v>31</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>156</v>
@@ -4955,36 +4955,36 @@
         <v>26</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>98</v>
+      <c r="B51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>157</v>
@@ -5001,10 +5001,10 @@
         <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>157</v>
@@ -5015,7 +5015,7 @@
         <v>26</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>10</v>
@@ -5024,7 +5024,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>158</v>
@@ -5035,16 +5035,16 @@
         <v>33</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>158</v>
@@ -5055,16 +5055,16 @@
         <v>29</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>158</v>
@@ -5183,8 +5183,8 @@
       <c r="F69" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A1:F55">
-    <sortCondition ref="F1:F55"/>
+  <sortState ref="A1:F69">
+    <sortCondition ref="F1:F69"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>